<commit_message>
status report 3 + timesheet
</commit_message>
<xml_diff>
--- a/timesheets/ash/timesheet.xlsx
+++ b/timesheets/ash/timesheet.xlsx
@@ -1,20 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11008"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ash/Desktop/Boulder/Fa23 Classes/canopy/admin/timesheets/ash/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E476DEBE-67CB-204B-96DF-B4A18CE4260E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B353B3B2-D9E3-654F-8669-2924909A651F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20940" yWindow="-21100" windowWidth="34560" windowHeight="18240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20940" yWindow="-21100" windowWidth="34560" windowHeight="18240" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Week1" sheetId="1" r:id="rId1"/>
     <sheet name="Week2" sheetId="2" r:id="rId2"/>
+    <sheet name="Week3" sheetId="3" r:id="rId3"/>
+    <sheet name="Week4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="29">
   <si>
     <t>Name</t>
   </si>
@@ -115,13 +117,22 @@
   </si>
   <si>
     <t>Fix mem leak</t>
+  </si>
+  <si>
+    <t>Tree refactor</t>
+  </si>
+  <si>
+    <t>Research</t>
+  </si>
+  <si>
+    <t>Initial sphere</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -145,8 +156,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -177,8 +203,32 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFCE4D6"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9E1F2"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE2EFDA"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE7E6E6"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -214,12 +264,69 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -237,6 +344,37 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="3" fillId="7" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="3" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -879,8 +1017,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FA69E54-CD6F-0D40-8020-0309A48E2F1E}">
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView zoomScale="125" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -973,10 +1111,10 @@
         <v>7</v>
       </c>
       <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1">
-        <v>1</v>
-      </c>
+      <c r="C6" s="1">
+        <v>1</v>
+      </c>
+      <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
@@ -1154,11 +1292,11 @@
       </c>
       <c r="C16" s="4">
         <f t="shared" ref="C16:H16" si="1">SUM(C6:C15)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D16" s="4">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E16" s="4">
         <f t="shared" si="1"/>
@@ -1215,6 +1353,801 @@
       <c r="A24" s="5" t="s">
         <v>15</v>
       </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="B4:H4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0D8A3C3-5B90-D540-8EEA-C4DA06E1BB95}">
+  <dimension ref="A1:I24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B16" sqref="B16:H16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="8"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="8"/>
+      <c r="B4" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="8"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="10">
+        <v>45207</v>
+      </c>
+      <c r="C5" s="10">
+        <v>45208</v>
+      </c>
+      <c r="D5" s="10">
+        <v>45209</v>
+      </c>
+      <c r="E5" s="10">
+        <v>45210</v>
+      </c>
+      <c r="F5" s="10">
+        <v>45211</v>
+      </c>
+      <c r="G5" s="10">
+        <v>45212</v>
+      </c>
+      <c r="H5" s="11">
+        <v>45213</v>
+      </c>
+      <c r="I5" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1">
+        <v>1</v>
+      </c>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="4">
+        <f t="shared" ref="I6:I15" si="0">SUM(B6:H6)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1">
+        <v>1</v>
+      </c>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="4">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1">
+        <v>1</v>
+      </c>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="4">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1">
+        <v>3</v>
+      </c>
+      <c r="G10" s="1"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="4">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1">
+        <v>1</v>
+      </c>
+      <c r="F11" s="1">
+        <v>2</v>
+      </c>
+      <c r="G11" s="1">
+        <v>2</v>
+      </c>
+      <c r="H11" s="3"/>
+      <c r="I11" s="4">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="3">
+        <v>2</v>
+      </c>
+      <c r="I12" s="4">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16" s="4">
+        <f>SUM(B6:B15)</f>
+        <v>0</v>
+      </c>
+      <c r="C16" s="4">
+        <f t="shared" ref="C16:H16" si="1">SUM(C6:C15)</f>
+        <v>2</v>
+      </c>
+      <c r="D16" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E16" s="4">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="F16" s="4">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="G16" s="4">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="H16" s="4">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="I16" s="4">
+        <f>SUM(I6:I15)</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="B4:H4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCA61B5E-74A1-C848-BB99-4E2B67622939}">
+  <dimension ref="A1:J24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="28"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="17"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="28"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="17"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="16"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16"/>
+      <c r="I3" s="16"/>
+      <c r="J3" s="17"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="16"/>
+      <c r="B4" s="31" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="33"/>
+      <c r="I4" s="16"/>
+      <c r="J4" s="17"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="20">
+        <v>45214</v>
+      </c>
+      <c r="C5" s="20">
+        <v>45215</v>
+      </c>
+      <c r="D5" s="20">
+        <v>45216</v>
+      </c>
+      <c r="E5" s="20">
+        <v>45217</v>
+      </c>
+      <c r="F5" s="20">
+        <v>45218</v>
+      </c>
+      <c r="G5" s="20">
+        <v>45219</v>
+      </c>
+      <c r="H5" s="21">
+        <v>45220</v>
+      </c>
+      <c r="I5" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="J5" s="17"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="24"/>
+      <c r="C6" s="24">
+        <v>1</v>
+      </c>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="25"/>
+      <c r="I6" s="4">
+        <f t="shared" ref="I6:I15" si="0">SUM(B6:H6)</f>
+        <v>1</v>
+      </c>
+      <c r="J6" s="17"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="24"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="24"/>
+      <c r="F7" s="24"/>
+      <c r="G7" s="24"/>
+      <c r="H7" s="25"/>
+      <c r="I7" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J7" s="17"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="24"/>
+      <c r="C8" s="24">
+        <v>1</v>
+      </c>
+      <c r="D8" s="24"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="24"/>
+      <c r="H8" s="25"/>
+      <c r="I8" s="4">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="J8" s="17"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="24"/>
+      <c r="C9" s="24"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="24">
+        <v>1</v>
+      </c>
+      <c r="F9" s="24"/>
+      <c r="G9" s="24"/>
+      <c r="H9" s="25"/>
+      <c r="I9" s="4">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="J9" s="17"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="24"/>
+      <c r="C10" s="24"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="24">
+        <v>2</v>
+      </c>
+      <c r="F10" s="24">
+        <v>2</v>
+      </c>
+      <c r="G10" s="24"/>
+      <c r="H10" s="25"/>
+      <c r="I10" s="4">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="J10" s="17"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="24"/>
+      <c r="C11" s="24"/>
+      <c r="D11" s="24">
+        <v>2</v>
+      </c>
+      <c r="E11" s="24">
+        <v>2</v>
+      </c>
+      <c r="F11" s="24"/>
+      <c r="G11" s="24"/>
+      <c r="H11" s="25"/>
+      <c r="I11" s="4">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="J11" s="17"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="24"/>
+      <c r="C12" s="24"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="24"/>
+      <c r="F12" s="24"/>
+      <c r="G12" s="24">
+        <v>2</v>
+      </c>
+      <c r="H12" s="25">
+        <v>2</v>
+      </c>
+      <c r="I12" s="4">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="J12" s="17"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="24"/>
+      <c r="C13" s="24"/>
+      <c r="D13" s="24"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="24"/>
+      <c r="G13" s="24"/>
+      <c r="H13" s="25"/>
+      <c r="I13" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J13" s="17"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" s="24"/>
+      <c r="C14" s="24"/>
+      <c r="D14" s="24"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="24"/>
+      <c r="G14" s="24"/>
+      <c r="H14" s="25"/>
+      <c r="I14" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J14" s="17"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="24"/>
+      <c r="C15" s="24"/>
+      <c r="D15" s="24"/>
+      <c r="E15" s="24"/>
+      <c r="F15" s="24"/>
+      <c r="G15" s="24"/>
+      <c r="H15" s="25"/>
+      <c r="I15" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J15" s="17"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16" s="4">
+        <f>SUM(B6:B15)</f>
+        <v>0</v>
+      </c>
+      <c r="C16" s="4">
+        <f t="shared" ref="C16:H16" si="1">SUM(C6:C15)</f>
+        <v>2</v>
+      </c>
+      <c r="D16" s="4">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="E16" s="4">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="F16" s="4">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="G16" s="4">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="H16" s="4">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="I16" s="4">
+        <f>SUM(I6:I15)</f>
+        <v>15</v>
+      </c>
+      <c r="J16" s="17"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A17" s="17"/>
+      <c r="B17" s="17"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="17"/>
+      <c r="G17" s="17"/>
+      <c r="H17" s="17"/>
+      <c r="I17" s="17"/>
+      <c r="J17" s="17"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A18" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" s="27"/>
+      <c r="C18" s="27"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="17"/>
+      <c r="F18" s="17"/>
+      <c r="G18" s="17"/>
+      <c r="H18" s="17"/>
+      <c r="I18" s="17"/>
+      <c r="J18" s="17"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A19" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19" s="27"/>
+      <c r="C19" s="27"/>
+      <c r="D19" s="17"/>
+      <c r="E19" s="17"/>
+      <c r="F19" s="17"/>
+      <c r="G19" s="17"/>
+      <c r="H19" s="17"/>
+      <c r="I19" s="17"/>
+      <c r="J19" s="17"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A20" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="B20" s="27"/>
+      <c r="C20" s="27"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="17"/>
+      <c r="F20" s="17"/>
+      <c r="G20" s="17"/>
+      <c r="H20" s="17"/>
+      <c r="I20" s="17"/>
+      <c r="J20" s="17"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A21" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="B21" s="27"/>
+      <c r="C21" s="27"/>
+      <c r="D21" s="27"/>
+      <c r="E21" s="17"/>
+      <c r="F21" s="17"/>
+      <c r="G21" s="17"/>
+      <c r="H21" s="17"/>
+      <c r="I21" s="17"/>
+      <c r="J21" s="17"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A22" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="B22" s="27"/>
+      <c r="C22" s="27"/>
+      <c r="D22" s="27"/>
+      <c r="E22" s="27"/>
+      <c r="F22" s="27"/>
+      <c r="G22" s="17"/>
+      <c r="H22" s="17"/>
+      <c r="I22" s="17"/>
+      <c r="J22" s="17"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A23" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" s="27"/>
+      <c r="C23" s="27"/>
+      <c r="D23" s="27"/>
+      <c r="E23" s="27"/>
+      <c r="F23" s="27"/>
+      <c r="G23" s="27"/>
+      <c r="H23" s="27"/>
+      <c r="I23" s="17"/>
+      <c r="J23" s="17"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A24" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="B24" s="27"/>
+      <c r="C24" s="27"/>
+      <c r="D24" s="27"/>
+      <c r="E24" s="27"/>
+      <c r="F24" s="27"/>
+      <c r="G24" s="17"/>
+      <c r="H24" s="17"/>
+      <c r="I24" s="17"/>
+      <c r="J24" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
requirements doc + weekly ash stuff
</commit_message>
<xml_diff>
--- a/timesheets/ash/timesheet.xlsx
+++ b/timesheets/ash/timesheet.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ash/Desktop/Boulder/Fa23 Classes/canopy/admin/timesheets/ash/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B353B3B2-D9E3-654F-8669-2924909A651F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A38D6551-CF9A-1D4F-91AF-E71AEC8E3F7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20940" yWindow="-21100" windowWidth="34560" windowHeight="18240" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20360" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Week1" sheetId="1" r:id="rId1"/>
     <sheet name="Week2" sheetId="2" r:id="rId2"/>
     <sheet name="Week3" sheetId="3" r:id="rId3"/>
     <sheet name="Week4" sheetId="4" r:id="rId4"/>
+    <sheet name="Week5" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="30">
   <si>
     <t>Name</t>
   </si>
@@ -126,6 +127,9 @@
   </si>
   <si>
     <t>Initial sphere</t>
+  </si>
+  <si>
+    <t>*3 midterms this week, less time than usual</t>
   </si>
 </sst>
 </file>
@@ -340,12 +344,6 @@
     <xf numFmtId="16" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="16" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -359,10 +357,16 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -676,11 +680,11 @@
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
       <c r="E1" s="8"/>
       <c r="F1" s="8"/>
       <c r="G1" s="8"/>
@@ -691,11 +695,11 @@
       <c r="A2" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
       <c r="G2" s="8"/>
@@ -715,15 +719,15 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="8"/>
-      <c r="B4" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
+      <c r="B4" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
       <c r="I4" s="8"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -1027,11 +1031,11 @@
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
       <c r="E1" s="8"/>
       <c r="F1" s="8"/>
       <c r="G1" s="8"/>
@@ -1042,11 +1046,11 @@
       <c r="A2" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
       <c r="G2" s="8"/>
@@ -1066,15 +1070,15 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="8"/>
-      <c r="B4" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
+      <c r="B4" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
       <c r="I4" s="8"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -1378,11 +1382,11 @@
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
       <c r="E1" s="8"/>
       <c r="F1" s="8"/>
       <c r="G1" s="8"/>
@@ -1393,11 +1397,11 @@
       <c r="A2" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
       <c r="G2" s="8"/>
@@ -1417,15 +1421,15 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="8"/>
-      <c r="B4" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
+      <c r="B4" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
       <c r="I4" s="8"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -1719,58 +1723,58 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCA61B5E-74A1-C848-BB99-4E2B67622939}">
   <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="29" t="s">
+      <c r="A1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="28"/>
+      <c r="C1" s="29"/>
       <c r="D1" s="30"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="17"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="15"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="28"/>
+      <c r="C2" s="29"/>
       <c r="D2" s="30"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="17"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="15"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" s="16"/>
-      <c r="B3" s="16"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="16"/>
-      <c r="H3" s="16"/>
-      <c r="I3" s="16"/>
-      <c r="J3" s="17"/>
+      <c r="A3" s="14"/>
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="15"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" s="16"/>
+      <c r="A4" s="14"/>
       <c r="B4" s="31" t="s">
         <v>1</v>
       </c>
@@ -1780,229 +1784,229 @@
       <c r="F4" s="32"/>
       <c r="G4" s="32"/>
       <c r="H4" s="33"/>
-      <c r="I4" s="16"/>
-      <c r="J4" s="17"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="15"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="20">
+      <c r="A5" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="18">
         <v>45214</v>
       </c>
-      <c r="C5" s="20">
+      <c r="C5" s="18">
         <v>45215</v>
       </c>
-      <c r="D5" s="20">
+      <c r="D5" s="18">
         <v>45216</v>
       </c>
-      <c r="E5" s="20">
+      <c r="E5" s="18">
         <v>45217</v>
       </c>
-      <c r="F5" s="20">
+      <c r="F5" s="18">
         <v>45218</v>
       </c>
-      <c r="G5" s="20">
+      <c r="G5" s="18">
         <v>45219</v>
       </c>
-      <c r="H5" s="21">
+      <c r="H5" s="19">
         <v>45220</v>
       </c>
-      <c r="I5" s="22" t="s">
+      <c r="I5" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="J5" s="17"/>
+      <c r="J5" s="15"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A6" s="23" t="s">
+      <c r="A6" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="24"/>
-      <c r="C6" s="24">
-        <v>1</v>
-      </c>
-      <c r="D6" s="24"/>
-      <c r="E6" s="24"/>
-      <c r="F6" s="24"/>
-      <c r="G6" s="24"/>
-      <c r="H6" s="25"/>
+      <c r="B6" s="22"/>
+      <c r="C6" s="22">
+        <v>1</v>
+      </c>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="22"/>
+      <c r="G6" s="22"/>
+      <c r="H6" s="23"/>
       <c r="I6" s="4">
         <f t="shared" ref="I6:I15" si="0">SUM(B6:H6)</f>
         <v>1</v>
       </c>
-      <c r="J6" s="17"/>
+      <c r="J6" s="15"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A7" s="23" t="s">
+      <c r="A7" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="24"/>
-      <c r="C7" s="24"/>
-      <c r="D7" s="24"/>
-      <c r="E7" s="24"/>
-      <c r="F7" s="24"/>
-      <c r="G7" s="24"/>
-      <c r="H7" s="25"/>
+      <c r="B7" s="22"/>
+      <c r="C7" s="22"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="22"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="23"/>
       <c r="I7" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J7" s="17"/>
+      <c r="J7" s="15"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A8" s="23" t="s">
+      <c r="A8" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="24"/>
-      <c r="C8" s="24">
-        <v>1</v>
-      </c>
-      <c r="D8" s="24"/>
-      <c r="E8" s="24"/>
-      <c r="F8" s="24"/>
-      <c r="G8" s="24"/>
-      <c r="H8" s="25"/>
+      <c r="B8" s="22"/>
+      <c r="C8" s="22">
+        <v>1</v>
+      </c>
+      <c r="D8" s="22"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="22"/>
+      <c r="H8" s="23"/>
       <c r="I8" s="4">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="J8" s="17"/>
+      <c r="J8" s="15"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A9" s="23" t="s">
+      <c r="A9" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="24"/>
-      <c r="C9" s="24"/>
-      <c r="D9" s="24"/>
-      <c r="E9" s="24">
-        <v>1</v>
-      </c>
-      <c r="F9" s="24"/>
-      <c r="G9" s="24"/>
-      <c r="H9" s="25"/>
+      <c r="B9" s="22"/>
+      <c r="C9" s="22"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="22">
+        <v>1</v>
+      </c>
+      <c r="F9" s="22"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="23"/>
       <c r="I9" s="4">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="J9" s="17"/>
+      <c r="J9" s="15"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A10" s="23" t="s">
+      <c r="A10" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="B10" s="24"/>
-      <c r="C10" s="24"/>
-      <c r="D10" s="24"/>
-      <c r="E10" s="24">
-        <v>2</v>
-      </c>
-      <c r="F10" s="24">
-        <v>2</v>
-      </c>
-      <c r="G10" s="24"/>
-      <c r="H10" s="25"/>
+      <c r="B10" s="22"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="22">
+        <v>2</v>
+      </c>
+      <c r="F10" s="22">
+        <v>2</v>
+      </c>
+      <c r="G10" s="22"/>
+      <c r="H10" s="23"/>
       <c r="I10" s="4">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="J10" s="17"/>
+      <c r="J10" s="15"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A11" s="23" t="s">
+      <c r="A11" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="24"/>
-      <c r="C11" s="24"/>
-      <c r="D11" s="24">
-        <v>2</v>
-      </c>
-      <c r="E11" s="24">
-        <v>2</v>
-      </c>
-      <c r="F11" s="24"/>
-      <c r="G11" s="24"/>
-      <c r="H11" s="25"/>
+      <c r="B11" s="22"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="22">
+        <v>2</v>
+      </c>
+      <c r="E11" s="22">
+        <v>2</v>
+      </c>
+      <c r="F11" s="22"/>
+      <c r="G11" s="22"/>
+      <c r="H11" s="23"/>
       <c r="I11" s="4">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="J11" s="17"/>
+      <c r="J11" s="15"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A12" s="23" t="s">
+      <c r="A12" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="24"/>
-      <c r="C12" s="24"/>
-      <c r="D12" s="24"/>
-      <c r="E12" s="24"/>
-      <c r="F12" s="24"/>
-      <c r="G12" s="24">
-        <v>2</v>
-      </c>
-      <c r="H12" s="25">
+      <c r="B12" s="22"/>
+      <c r="C12" s="22"/>
+      <c r="D12" s="22"/>
+      <c r="E12" s="22"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="22">
+        <v>2</v>
+      </c>
+      <c r="H12" s="23">
         <v>2</v>
       </c>
       <c r="I12" s="4">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="J12" s="17"/>
+      <c r="J12" s="15"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A13" s="23" t="s">
+      <c r="A13" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="24"/>
-      <c r="C13" s="24"/>
-      <c r="D13" s="24"/>
-      <c r="E13" s="24"/>
-      <c r="F13" s="24"/>
-      <c r="G13" s="24"/>
-      <c r="H13" s="25"/>
+      <c r="B13" s="22"/>
+      <c r="C13" s="22"/>
+      <c r="D13" s="22"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="22"/>
+      <c r="G13" s="22"/>
+      <c r="H13" s="23"/>
       <c r="I13" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J13" s="17"/>
+      <c r="J13" s="15"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A14" s="23" t="s">
+      <c r="A14" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="24"/>
-      <c r="C14" s="24"/>
-      <c r="D14" s="24"/>
-      <c r="E14" s="24"/>
-      <c r="F14" s="24"/>
-      <c r="G14" s="24"/>
-      <c r="H14" s="25"/>
+      <c r="B14" s="22"/>
+      <c r="C14" s="22"/>
+      <c r="D14" s="22"/>
+      <c r="E14" s="22"/>
+      <c r="F14" s="22"/>
+      <c r="G14" s="22"/>
+      <c r="H14" s="23"/>
       <c r="I14" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J14" s="17"/>
+      <c r="J14" s="15"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A15" s="23" t="s">
+      <c r="A15" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="24"/>
-      <c r="C15" s="24"/>
-      <c r="D15" s="24"/>
-      <c r="E15" s="24"/>
-      <c r="F15" s="24"/>
-      <c r="G15" s="24"/>
-      <c r="H15" s="25"/>
+      <c r="B15" s="22"/>
+      <c r="C15" s="22"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="22"/>
+      <c r="F15" s="22"/>
+      <c r="G15" s="22"/>
+      <c r="H15" s="23"/>
       <c r="I15" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J15" s="17"/>
+      <c r="J15" s="15"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A16" s="26" t="s">
+      <c r="A16" s="24" t="s">
         <v>3</v>
       </c>
       <c r="B16" s="4">
@@ -2037,117 +2041,535 @@
         <f>SUM(I6:I15)</f>
         <v>15</v>
       </c>
-      <c r="J16" s="17"/>
+      <c r="J16" s="15"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A17" s="17"/>
-      <c r="B17" s="17"/>
-      <c r="C17" s="17"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="17"/>
-      <c r="G17" s="17"/>
-      <c r="H17" s="17"/>
-      <c r="I17" s="17"/>
-      <c r="J17" s="17"/>
+      <c r="A17" s="15"/>
+      <c r="B17" s="15"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="15"/>
+      <c r="H17" s="15"/>
+      <c r="I17" s="15"/>
+      <c r="J17" s="15"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A18" s="27" t="s">
+      <c r="A18" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="27"/>
-      <c r="C18" s="27"/>
-      <c r="D18" s="17"/>
-      <c r="E18" s="17"/>
-      <c r="F18" s="17"/>
-      <c r="G18" s="17"/>
-      <c r="H18" s="17"/>
-      <c r="I18" s="17"/>
-      <c r="J18" s="17"/>
+      <c r="B18" s="25"/>
+      <c r="C18" s="25"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="15"/>
+      <c r="H18" s="15"/>
+      <c r="I18" s="15"/>
+      <c r="J18" s="15"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A19" s="27" t="s">
+      <c r="A19" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="B19" s="27"/>
-      <c r="C19" s="27"/>
-      <c r="D19" s="17"/>
-      <c r="E19" s="17"/>
-      <c r="F19" s="17"/>
-      <c r="G19" s="17"/>
-      <c r="H19" s="17"/>
-      <c r="I19" s="17"/>
-      <c r="J19" s="17"/>
+      <c r="B19" s="25"/>
+      <c r="C19" s="25"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="15"/>
+      <c r="H19" s="15"/>
+      <c r="I19" s="15"/>
+      <c r="J19" s="15"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A20" s="27" t="s">
+      <c r="A20" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="B20" s="27"/>
-      <c r="C20" s="27"/>
-      <c r="D20" s="17"/>
-      <c r="E20" s="17"/>
-      <c r="F20" s="17"/>
-      <c r="G20" s="17"/>
-      <c r="H20" s="17"/>
-      <c r="I20" s="17"/>
-      <c r="J20" s="17"/>
+      <c r="B20" s="25"/>
+      <c r="C20" s="25"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="15"/>
+      <c r="G20" s="15"/>
+      <c r="H20" s="15"/>
+      <c r="I20" s="15"/>
+      <c r="J20" s="15"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A21" s="27" t="s">
+      <c r="A21" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="B21" s="27"/>
-      <c r="C21" s="27"/>
-      <c r="D21" s="27"/>
-      <c r="E21" s="17"/>
-      <c r="F21" s="17"/>
-      <c r="G21" s="17"/>
-      <c r="H21" s="17"/>
-      <c r="I21" s="17"/>
-      <c r="J21" s="17"/>
+      <c r="B21" s="25"/>
+      <c r="C21" s="25"/>
+      <c r="D21" s="25"/>
+      <c r="E21" s="15"/>
+      <c r="F21" s="15"/>
+      <c r="G21" s="15"/>
+      <c r="H21" s="15"/>
+      <c r="I21" s="15"/>
+      <c r="J21" s="15"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A22" s="27" t="s">
+      <c r="A22" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="B22" s="27"/>
-      <c r="C22" s="27"/>
-      <c r="D22" s="27"/>
-      <c r="E22" s="27"/>
-      <c r="F22" s="27"/>
-      <c r="G22" s="17"/>
-      <c r="H22" s="17"/>
-      <c r="I22" s="17"/>
-      <c r="J22" s="17"/>
+      <c r="B22" s="25"/>
+      <c r="C22" s="25"/>
+      <c r="D22" s="25"/>
+      <c r="E22" s="25"/>
+      <c r="F22" s="25"/>
+      <c r="G22" s="15"/>
+      <c r="H22" s="15"/>
+      <c r="I22" s="15"/>
+      <c r="J22" s="15"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A23" s="27" t="s">
+      <c r="A23" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="B23" s="27"/>
-      <c r="C23" s="27"/>
-      <c r="D23" s="27"/>
-      <c r="E23" s="27"/>
-      <c r="F23" s="27"/>
-      <c r="G23" s="27"/>
-      <c r="H23" s="27"/>
-      <c r="I23" s="17"/>
-      <c r="J23" s="17"/>
+      <c r="B23" s="25"/>
+      <c r="C23" s="25"/>
+      <c r="D23" s="25"/>
+      <c r="E23" s="25"/>
+      <c r="F23" s="25"/>
+      <c r="G23" s="25"/>
+      <c r="H23" s="25"/>
+      <c r="I23" s="15"/>
+      <c r="J23" s="15"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A24" s="27" t="s">
+      <c r="A24" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="B24" s="27"/>
-      <c r="C24" s="27"/>
-      <c r="D24" s="27"/>
-      <c r="E24" s="27"/>
-      <c r="F24" s="27"/>
-      <c r="G24" s="17"/>
-      <c r="H24" s="17"/>
-      <c r="I24" s="17"/>
-      <c r="J24" s="17"/>
+      <c r="B24" s="25"/>
+      <c r="C24" s="25"/>
+      <c r="D24" s="25"/>
+      <c r="E24" s="25"/>
+      <c r="F24" s="25"/>
+      <c r="G24" s="15"/>
+      <c r="H24" s="15"/>
+      <c r="I24" s="15"/>
+      <c r="J24" s="15"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="B4:H4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8516C1E9-394C-FE4B-B7FE-11D5BFF17952}">
+  <dimension ref="A1:I24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="29"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="29"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="14"/>
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="14"/>
+      <c r="B4" s="31" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="33"/>
+      <c r="I4" s="14"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="18">
+        <v>45221</v>
+      </c>
+      <c r="C5" s="18">
+        <v>45222</v>
+      </c>
+      <c r="D5" s="18">
+        <v>45223</v>
+      </c>
+      <c r="E5" s="18">
+        <v>45224</v>
+      </c>
+      <c r="F5" s="18">
+        <v>45225</v>
+      </c>
+      <c r="G5" s="18">
+        <v>45226</v>
+      </c>
+      <c r="H5" s="19">
+        <v>45227</v>
+      </c>
+      <c r="I5" s="20" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="22"/>
+      <c r="C6" s="22">
+        <v>1</v>
+      </c>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="22"/>
+      <c r="G6" s="22"/>
+      <c r="H6" s="23"/>
+      <c r="I6" s="4">
+        <f t="shared" ref="I6:I15" si="0">SUM(B6:H6)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="22"/>
+      <c r="C7" s="22"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="22"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="23"/>
+      <c r="I7" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="22"/>
+      <c r="C8" s="22">
+        <v>1</v>
+      </c>
+      <c r="D8" s="22"/>
+      <c r="E8" s="22">
+        <v>1</v>
+      </c>
+      <c r="F8" s="22"/>
+      <c r="G8" s="22"/>
+      <c r="H8" s="23"/>
+      <c r="I8" s="4">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="22"/>
+      <c r="C9" s="22"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="22">
+        <v>1</v>
+      </c>
+      <c r="F9" s="22"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="23"/>
+      <c r="I9" s="4">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="22"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="22">
+        <v>2</v>
+      </c>
+      <c r="G10" s="22"/>
+      <c r="H10" s="23"/>
+      <c r="I10" s="4">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="22"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="22"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="22">
+        <v>2</v>
+      </c>
+      <c r="G11" s="22"/>
+      <c r="H11" s="23"/>
+      <c r="I11" s="4">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="22"/>
+      <c r="C12" s="22"/>
+      <c r="D12" s="22"/>
+      <c r="E12" s="22"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="22"/>
+      <c r="H12" s="23">
+        <v>2</v>
+      </c>
+      <c r="I12" s="4">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="22"/>
+      <c r="C13" s="22"/>
+      <c r="D13" s="22"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="22"/>
+      <c r="G13" s="22"/>
+      <c r="H13" s="23"/>
+      <c r="I13" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" s="22"/>
+      <c r="C14" s="22"/>
+      <c r="D14" s="22"/>
+      <c r="E14" s="22"/>
+      <c r="F14" s="22"/>
+      <c r="G14" s="22"/>
+      <c r="H14" s="23"/>
+      <c r="I14" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="22"/>
+      <c r="C15" s="22"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="22"/>
+      <c r="F15" s="22"/>
+      <c r="G15" s="22"/>
+      <c r="H15" s="23"/>
+      <c r="I15" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16" s="4">
+        <f>SUM(B6:B15)</f>
+        <v>0</v>
+      </c>
+      <c r="C16" s="4">
+        <f t="shared" ref="C16:H16" si="1">SUM(C6:C15)</f>
+        <v>2</v>
+      </c>
+      <c r="D16" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E16" s="4">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="F16" s="4">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="G16" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H16" s="4">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="I16" s="4">
+        <f>SUM(I6:I15)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" s="15"/>
+      <c r="B17" s="15"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="15"/>
+      <c r="H17" s="15"/>
+      <c r="I17" s="15"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" s="25"/>
+      <c r="C18" s="25"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="15"/>
+      <c r="H18" s="15"/>
+      <c r="I18" s="15"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19" s="25"/>
+      <c r="C19" s="25"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="15"/>
+      <c r="H19" s="15"/>
+      <c r="I19" s="15"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="B20" s="25"/>
+      <c r="C20" s="25"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="15"/>
+      <c r="G20" s="15"/>
+      <c r="H20" s="15"/>
+      <c r="I20" s="15"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="B21" s="25"/>
+      <c r="C21" s="25"/>
+      <c r="D21" s="25"/>
+      <c r="E21" s="15"/>
+      <c r="F21" s="15"/>
+      <c r="G21" s="15"/>
+      <c r="H21" s="15"/>
+      <c r="I21" s="15"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="B22" s="25"/>
+      <c r="C22" s="25"/>
+      <c r="D22" s="25"/>
+      <c r="E22" s="25"/>
+      <c r="F22" s="25"/>
+      <c r="G22" s="15"/>
+      <c r="H22" s="15"/>
+      <c r="I22" s="15"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" s="25"/>
+      <c r="C23" s="25"/>
+      <c r="D23" s="25"/>
+      <c r="E23" s="25"/>
+      <c r="F23" s="25"/>
+      <c r="G23" s="25"/>
+      <c r="H23" s="25"/>
+      <c r="I23" s="15"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="B24" s="25"/>
+      <c r="C24" s="25"/>
+      <c r="D24" s="25"/>
+      <c r="E24" s="25"/>
+      <c r="F24" s="25"/>
+      <c r="G24" s="15"/>
+      <c r="H24" s="15"/>
+      <c r="I24" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>